<commit_message>
Added models to list
Added models to list --> also might not look at GPT-3 and GPT-2
</commit_message>
<xml_diff>
--- a/data/LLM Matrix.xlsx
+++ b/data/LLM Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>model</t>
   </si>
@@ -127,6 +127,33 @@
   </si>
   <si>
     <t>Percieved Business Value --&gt; y-axis</t>
+  </si>
+  <si>
+    <t>GPT-J</t>
+  </si>
+  <si>
+    <t>EleutherAI</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Megatron-LM</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>BLOOM</t>
+  </si>
+  <si>
+    <t>BigScience</t>
+  </si>
+  <si>
+    <t>ERNIE 4.0</t>
+  </si>
+  <si>
+    <t>Baidu</t>
   </si>
 </sst>
 </file>
@@ -620,7 +647,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -636,9 +663,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1123,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1132,12 +1156,12 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="11.26953125" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" customWidth="1"/>
-    <col min="4" max="5" width="12.36328125" style="15" customWidth="1"/>
+    <col min="4" max="5" width="12.36328125" style="14" customWidth="1"/>
     <col min="6" max="6" width="13.90625" customWidth="1"/>
-    <col min="7" max="9" width="13.90625" style="15" customWidth="1"/>
+    <col min="7" max="9" width="13.90625" style="14" customWidth="1"/>
     <col min="10" max="10" width="16.1796875" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" customWidth="1"/>
-    <col min="12" max="17" width="11.26953125" style="15" customWidth="1"/>
+    <col min="12" max="17" width="11.26953125" style="14" customWidth="1"/>
     <col min="18" max="18" width="13.26953125" customWidth="1"/>
     <col min="19" max="19" width="13.26953125" style="1" customWidth="1"/>
     <col min="20" max="20" width="14.26953125" customWidth="1"/>
@@ -1148,56 +1172,56 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="6"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="6"/>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
       <c r="S2" s="6"/>
       <c r="W2" s="6"/>
     </row>
@@ -1279,7 +1303,7 @@
       <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>44999</v>
       </c>
       <c r="D4" s="2">
@@ -1415,10 +1439,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>45400</v>
       </c>
       <c r="D7" s="2"/>
@@ -1476,7 +1500,15 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="D9" s="2"/>
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15">
+        <v>43761</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1499,9 +1531,15 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="B10" s="11"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="15">
+        <v>44351</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1524,7 +1562,15 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="D11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="15">
+        <v>44295</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1547,7 +1593,15 @@
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="D12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="15">
+        <v>44754</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1570,7 +1624,15 @@
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="D13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="15">
+        <v>45216</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>

</xml_diff>

<commit_message>
LLM Matrix Update (5/6)
Added two more models to the Matrix. Also move the .ipyub file from 'data' to 'dataAnalysis'
</commit_message>
<xml_diff>
--- a/data/LLM Matrix.xlsx
+++ b/data/LLM Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Business Rediness - &gt; x-axis</t>
   </si>
@@ -199,6 +199,48 @@
   </si>
   <si>
     <t>SQuAD</t>
+  </si>
+  <si>
+    <t>General Purpose Model</t>
+  </si>
+  <si>
+    <t>specialisation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Specialised for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Financial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Tasks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Specialised for Manufacturing, Research, Finance and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Medicine. (Mainly known for Medicine and Research right now)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -208,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -219,6 +261,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -317,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -345,7 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -365,6 +412,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +461,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$4:$X$17</c:f>
+              <c:f>Sheet1!$Y$4:$Y$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="14"/>
@@ -447,7 +496,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2.9697747356321837</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -456,14 +505,14 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2.7490000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AE$4:$AE$17</c:f>
+              <c:f>Sheet1!$AF$4:$AF$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="14"/>
@@ -498,7 +547,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3.6945000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -507,7 +556,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1.9566666666666668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -668,7 +717,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -979,87 +1028,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM100"/>
+  <dimension ref="A1:AN100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="5" customWidth="1"/>
-    <col min="4" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="9" width="13.81640625" customWidth="1"/>
-    <col min="10" max="10" width="16.08984375" customWidth="1"/>
-    <col min="11" max="22" width="11.26953125" customWidth="1"/>
-    <col min="23" max="23" width="13.26953125" customWidth="1"/>
-    <col min="24" max="24" width="13.26953125" style="5" customWidth="1"/>
-    <col min="25" max="25" width="14.26953125" customWidth="1"/>
-    <col min="26" max="26" width="13.7265625" customWidth="1"/>
-    <col min="27" max="30" width="12.453125" customWidth="1"/>
-    <col min="31" max="31" width="8.7265625" style="5" customWidth="1"/>
-    <col min="32" max="39" width="8.7265625" customWidth="1"/>
+    <col min="2" max="3" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="5" customWidth="1"/>
+    <col min="5" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="10" width="13.81640625" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" customWidth="1"/>
+    <col min="12" max="23" width="11.26953125" customWidth="1"/>
+    <col min="24" max="24" width="13.26953125" customWidth="1"/>
+    <col min="25" max="25" width="13.26953125" style="5" customWidth="1"/>
+    <col min="26" max="26" width="14.26953125" customWidth="1"/>
+    <col min="27" max="27" width="13.7265625" customWidth="1"/>
+    <col min="28" max="31" width="12.453125" customWidth="1"/>
+    <col min="32" max="32" width="8.7265625" style="5" customWidth="1"/>
+    <col min="33" max="40" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:40" ht="14.25" customHeight="1" thickBot="1">
       <c r="A1" s="1"/>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="32" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="34"/>
-    </row>
-    <row r="2" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="33"/>
+    </row>
+    <row r="2" spans="1:40" ht="14.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="18" t="s">
+      <c r="J2" s="11"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="18" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
@@ -1067,235 +1115,242 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="22"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="28" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="21"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="22"/>
-    </row>
-    <row r="3" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="21"/>
+    </row>
+    <row r="3" spans="1:40" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="T3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="U3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="V3" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="W3" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="23" t="s">
+      <c r="Y3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="26" t="s">
+      <c r="Z3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="AA3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="30" t="s">
+      <c r="AB3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AC3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AD3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AE3" s="23" t="s">
+      <c r="AF3" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="14.25" customHeight="1">
+    <row r="4" spans="1:40" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="7">
         <v>44999</v>
       </c>
-      <c r="D4" s="20">
+      <c r="E4" s="20">
         <v>3</v>
       </c>
-      <c r="E4" s="13">
+      <c r="F4" s="13">
         <v>2</v>
       </c>
-      <c r="F4" s="13">
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="G4" s="14">
-        <f t="shared" ref="G4:G17" si="0">AVERAGE(D4,E4,F4)</f>
+      <c r="H4" s="14">
+        <f t="shared" ref="H4:H17" si="0">AVERAGE(E4,F4,G4)</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="H4" s="20">
+      <c r="I4" s="20">
         <v>2</v>
       </c>
-      <c r="I4" s="13">
+      <c r="J4" s="13">
         <v>3</v>
       </c>
-      <c r="J4" s="14">
-        <f t="shared" ref="J4:J17" si="1">AVERAGE(H4,I4)</f>
+      <c r="K4" s="14">
+        <f t="shared" ref="K4:K17" si="1">AVERAGE(I4,J4)</f>
         <v>2.5</v>
       </c>
-      <c r="K4" s="20">
+      <c r="L4" s="20">
         <f>AVERAGE(95.3, 86.4, 80.9, 35.7, 52.9, 67)%</f>
         <v>0.69700000000000006</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14">
-        <f>AVERAGE(K4:L4)*4</f>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14">
+        <f>AVERAGE(L4:M4)*4</f>
         <v>2.7880000000000003</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="13"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="13"/>
-      <c r="Q4" s="13">
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13">
         <v>0.91800000000000004</v>
       </c>
-      <c r="R4" s="13">
+      <c r="S4" s="13">
         <v>0.56799999999999995</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13">
+      <c r="T4" s="13"/>
+      <c r="U4" s="13">
         <v>0.79449999999999998</v>
       </c>
-      <c r="U4" s="13"/>
       <c r="V4" s="13"/>
-      <c r="W4" s="14">
-        <f>AVERAGE(N4,O4,P4,Q4,R4,S4,T4,U4,V4)*4</f>
+      <c r="W4" s="13"/>
+      <c r="X4" s="14">
+        <f>AVERAGE(O4,P4,Q4,R4,S4,T4,U4,V4,W4)*4</f>
         <v>3.0406666666666666</v>
       </c>
-      <c r="X4" s="24">
-        <f t="shared" ref="X4:X17" si="2">0.4*G4+0.3*J4+0.15*M4+0.15*W4</f>
+      <c r="Y4" s="23">
+        <f t="shared" ref="Y4:Y17" si="2">0.4*H4+0.3*K4+0.15*N4+0.15*X4</f>
         <v>2.6909666666666663</v>
       </c>
-      <c r="Y4" s="27">
+      <c r="Z4" s="26">
         <f>AVERAGE(4.5, 4.5, 3.5, 4, 3.5, 3.2, 4)/5*4</f>
         <v>3.1085714285714285</v>
       </c>
-      <c r="Z4" s="20">
+      <c r="AA4" s="20">
         <f>AVERAGE(4.7, 4, 3.5, 3.9)/5*4</f>
         <v>3.2199999999999998</v>
       </c>
-      <c r="AA4" s="31">
+      <c r="AB4" s="30">
         <v>4</v>
       </c>
-      <c r="AB4" s="13">
+      <c r="AC4" s="13">
         <v>4</v>
       </c>
-      <c r="AC4" s="13">
+      <c r="AD4" s="13">
         <v>3.5</v>
       </c>
-      <c r="AD4" s="14">
-        <f>AVERAGE(AA4:AC4)</f>
+      <c r="AE4" s="14">
+        <f>AVERAGE(AB4:AD4)</f>
         <v>3.8333333333333335</v>
       </c>
-      <c r="AE4" s="24">
-        <f>0.5*Y4+0.25*Z4+0.25*AD4</f>
+      <c r="AF4" s="23">
+        <f>0.5*Z4+0.25*AA4+0.25*AE4</f>
         <v>3.3176190476190475</v>
       </c>
-      <c r="AF4" s="4"/>
-    </row>
-    <row r="5" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG4" s="4"/>
+    </row>
+    <row r="5" spans="1:40" ht="14.25" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="1"/>
+      <c r="D5" s="7">
         <v>43993</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="14" t="e">
+      <c r="G5" s="13"/>
+      <c r="H5" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14" t="e">
+      <c r="I5" s="20"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14" t="e">
-        <f t="shared" ref="M5:M17" si="3">AVERAGE(K5:L5)*4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N5" s="20"/>
-      <c r="O5" s="13"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="14" t="e">
+        <f t="shared" ref="N5:N17" si="3">AVERAGE(L5:M5)*4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" s="20"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
@@ -1303,67 +1358,68 @@
       <c r="T5" s="13"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
-      <c r="W5" s="14" t="e">
-        <f t="shared" ref="W5:W17" si="4">AVERAGE(N5,O5,P5,Q5,R5,S5,T5,U5,V5)*4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X5" s="24" t="e">
+      <c r="W5" s="13"/>
+      <c r="X5" s="14" t="e">
+        <f t="shared" ref="X5:X17" si="4">AVERAGE(O5,P5,Q5,R5,S5,T5,U5,V5,W5)*4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y5" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="20"/>
+      <c r="Z5" s="26"/>
       <c r="AA5" s="20"/>
-      <c r="AB5" s="13"/>
+      <c r="AB5" s="20"/>
       <c r="AC5" s="13"/>
-      <c r="AD5" s="14" t="e">
-        <f t="shared" ref="AD5:AD17" si="5">AVERAGE(AA5:AC5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE5" s="24" t="e">
-        <f t="shared" ref="AE5:AE17" si="6">0.5*Y5+0.25*Z5+0.25*AD5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="1"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="14" t="e">
+        <f t="shared" ref="AE5:AE17" si="5">AVERAGE(AB5:AD5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF5" s="23" t="e">
+        <f t="shared" ref="AF5:AF17" si="6">0.5*Z5+0.25*AA5+0.25*AE5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG5" s="4"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
-    </row>
-    <row r="6" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AN5" s="1"/>
+    </row>
+    <row r="6" spans="1:40" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="1"/>
+      <c r="D6" s="7">
         <v>43770</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="14" t="e">
+      <c r="G6" s="13"/>
+      <c r="H6" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14" t="e">
+      <c r="I6" s="20"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14" t="e">
+      <c r="L6" s="20"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="20"/>
-      <c r="O6" s="13"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
@@ -1371,254 +1427,261 @@
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
-      <c r="W6" s="14" t="e">
+      <c r="W6" s="13"/>
+      <c r="X6" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X6" s="24" t="e">
+      <c r="Y6" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="20"/>
+      <c r="Z6" s="26"/>
       <c r="AA6" s="20"/>
-      <c r="AB6" s="13"/>
+      <c r="AB6" s="20"/>
       <c r="AC6" s="13"/>
-      <c r="AD6" s="14" t="e">
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE6" s="24" t="e">
+      <c r="AF6" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="1"/>
+      <c r="AG6" s="4"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
       <c r="AM6" s="1"/>
-    </row>
-    <row r="7" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AN6" s="1"/>
+    </row>
+    <row r="7" spans="1:40" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="7">
         <v>45400</v>
       </c>
-      <c r="D7" s="20">
+      <c r="E7" s="20">
         <v>2.7</v>
       </c>
-      <c r="E7" s="15">
+      <c r="F7" s="15">
         <v>1.2</v>
       </c>
-      <c r="F7" s="15">
+      <c r="G7" s="15">
         <v>1</v>
       </c>
-      <c r="G7" s="14">
+      <c r="H7" s="14">
         <f t="shared" si="0"/>
         <v>1.6333333333333335</v>
       </c>
-      <c r="H7" s="20">
+      <c r="I7" s="20">
         <v>3</v>
       </c>
-      <c r="I7" s="13">
+      <c r="J7" s="13">
         <v>3.7</v>
       </c>
-      <c r="J7" s="14">
+      <c r="K7" s="14">
         <f t="shared" si="1"/>
         <v>3.35</v>
       </c>
-      <c r="K7" s="20">
+      <c r="L7" s="20">
         <f>AVERAGE(85.6, 82, 79.7, 39.5, 30, 81.7)%</f>
         <v>0.66416666666666668</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14">
+      <c r="M7" s="13"/>
+      <c r="N7" s="14">
         <f t="shared" si="3"/>
         <v>2.6566666666666667</v>
       </c>
-      <c r="N7" s="20"/>
-      <c r="O7" s="13"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="13">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13">
         <v>0.84799999999999998</v>
       </c>
-      <c r="R7" s="13">
+      <c r="S7" s="13">
         <v>0.42699999999999999</v>
       </c>
-      <c r="S7" s="13">
+      <c r="T7" s="13">
         <v>0.36180000000000001</v>
       </c>
-      <c r="T7" s="13">
+      <c r="U7" s="13">
         <v>0.7923</v>
       </c>
-      <c r="U7" s="13"/>
       <c r="V7" s="13"/>
-      <c r="W7" s="14">
+      <c r="W7" s="13"/>
+      <c r="X7" s="14">
         <f t="shared" si="4"/>
         <v>2.4291</v>
       </c>
-      <c r="X7" s="24">
+      <c r="Y7" s="23">
         <f t="shared" si="2"/>
         <v>2.4211983333333329</v>
       </c>
-      <c r="Y7" s="27">
+      <c r="Z7" s="26">
         <v>3</v>
       </c>
-      <c r="Z7" s="20">
+      <c r="AA7" s="20">
         <v>2.5</v>
       </c>
-      <c r="AA7" s="20">
+      <c r="AB7" s="20">
         <v>4</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AC7" s="13">
         <v>4</v>
       </c>
-      <c r="AC7" s="13">
+      <c r="AD7" s="13">
         <v>3.7</v>
       </c>
-      <c r="AD7" s="14">
+      <c r="AE7" s="14">
         <f t="shared" si="5"/>
         <v>3.9</v>
       </c>
-      <c r="AE7" s="24">
+      <c r="AF7" s="23">
         <f t="shared" si="6"/>
         <v>3.1</v>
       </c>
-      <c r="AF7" s="4"/>
-    </row>
-    <row r="8" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG7" s="4"/>
+    </row>
+    <row r="8" spans="1:40" ht="14.25" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="7">
         <v>45266</v>
       </c>
-      <c r="D8" s="20">
+      <c r="E8" s="20">
         <f>3.8-1</f>
         <v>2.8</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <f>1.3-1</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="F8" s="13">
+      <c r="G8" s="13">
         <f>3.5-1</f>
         <v>2.5</v>
       </c>
-      <c r="G8" s="14">
+      <c r="H8" s="14">
         <f t="shared" si="0"/>
         <v>1.8666666666666665</v>
       </c>
-      <c r="H8" s="20">
+      <c r="I8" s="20">
         <f>1.5-1</f>
         <v>0.5</v>
       </c>
-      <c r="I8" s="13">
+      <c r="J8" s="13">
         <f>2-1</f>
         <v>1</v>
       </c>
-      <c r="J8" s="14">
+      <c r="K8" s="14">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="13">
+      <c r="L8" s="30"/>
+      <c r="M8" s="13">
         <v>0.63</v>
       </c>
-      <c r="M8" s="14">
+      <c r="N8" s="14">
         <f t="shared" si="3"/>
         <v>2.52</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="O8" s="13"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
-      <c r="V8" s="13">
+      <c r="V8" s="13"/>
+      <c r="W8" s="13">
         <v>0.49998999999999999</v>
       </c>
-      <c r="W8" s="14">
+      <c r="X8" s="14">
         <f t="shared" si="4"/>
         <v>1.99996</v>
       </c>
-      <c r="X8" s="24">
+      <c r="Y8" s="23">
         <f t="shared" si="2"/>
         <v>1.6496606666666667</v>
       </c>
-      <c r="Y8" s="27">
+      <c r="Z8" s="26">
         <f>4-1</f>
         <v>3</v>
       </c>
-      <c r="Z8" s="20">
+      <c r="AA8" s="20">
         <f>3.9-1</f>
         <v>2.9</v>
       </c>
-      <c r="AA8" s="20">
+      <c r="AB8" s="20">
         <f>2-1</f>
         <v>1</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AC8" s="13">
         <f>2-1</f>
         <v>1</v>
       </c>
-      <c r="AC8" s="13">
+      <c r="AD8" s="13">
         <f>3.2</f>
         <v>3.2</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AE8" s="14">
         <f t="shared" si="5"/>
         <v>1.7333333333333334</v>
       </c>
-      <c r="AE8" s="24">
+      <c r="AF8" s="23">
         <f t="shared" si="6"/>
         <v>2.6583333333333332</v>
       </c>
-      <c r="AF8" s="4"/>
-    </row>
-    <row r="9" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG8" s="4"/>
+    </row>
+    <row r="9" spans="1:40" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="1"/>
+      <c r="D9" s="7">
         <v>43761</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="14" t="e">
+      <c r="G9" s="13"/>
+      <c r="H9" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="14" t="e">
+      <c r="I9" s="30"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="14" t="e">
+      <c r="L9" s="30"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" s="20"/>
-      <c r="O9" s="13"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
@@ -1626,60 +1689,61 @@
       <c r="T9" s="13"/>
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
-      <c r="W9" s="14" t="e">
+      <c r="W9" s="13"/>
+      <c r="X9" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X9" s="24" t="e">
+      <c r="Y9" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="20"/>
+      <c r="Z9" s="26"/>
       <c r="AA9" s="20"/>
-      <c r="AB9" s="13"/>
+      <c r="AB9" s="20"/>
       <c r="AC9" s="13"/>
-      <c r="AD9" s="14" t="e">
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE9" s="24" t="e">
+      <c r="AF9" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF9" s="4"/>
-    </row>
-    <row r="10" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG9" s="4"/>
+    </row>
+    <row r="10" spans="1:40" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="1"/>
+      <c r="D10" s="7">
         <v>44351</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14" t="e">
+      <c r="E10" s="20"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14" t="e">
+      <c r="I10" s="20"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14" t="e">
+      <c r="L10" s="20"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="20"/>
-      <c r="O10" s="13"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
@@ -1687,60 +1751,61 @@
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
-      <c r="W10" s="14" t="e">
+      <c r="W10" s="13"/>
+      <c r="X10" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X10" s="24" t="e">
+      <c r="Y10" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="20"/>
+      <c r="Z10" s="26"/>
       <c r="AA10" s="20"/>
-      <c r="AB10" s="13"/>
+      <c r="AB10" s="20"/>
       <c r="AC10" s="13"/>
-      <c r="AD10" s="14" t="e">
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE10" s="24" t="e">
+      <c r="AF10" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF10" s="4"/>
-    </row>
-    <row r="11" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG10" s="4"/>
+    </row>
+    <row r="11" spans="1:40" ht="14.25" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="1"/>
+      <c r="D11" s="7">
         <v>44295</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="14" t="e">
+      <c r="G11" s="13"/>
+      <c r="H11" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14" t="e">
+      <c r="I11" s="20"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14" t="e">
+      <c r="L11" s="20"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="13"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
@@ -1748,60 +1813,61 @@
       <c r="T11" s="13"/>
       <c r="U11" s="13"/>
       <c r="V11" s="13"/>
-      <c r="W11" s="14" t="e">
+      <c r="W11" s="13"/>
+      <c r="X11" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X11" s="24" t="e">
+      <c r="Y11" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="20"/>
+      <c r="Z11" s="26"/>
       <c r="AA11" s="20"/>
-      <c r="AB11" s="13"/>
+      <c r="AB11" s="20"/>
       <c r="AC11" s="13"/>
-      <c r="AD11" s="14" t="e">
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE11" s="24" t="e">
+      <c r="AF11" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF11" s="4"/>
-    </row>
-    <row r="12" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG11" s="4"/>
+    </row>
+    <row r="12" spans="1:40" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="1"/>
+      <c r="D12" s="7">
         <v>44754</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="14" t="e">
+      <c r="G12" s="13"/>
+      <c r="H12" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14" t="e">
+      <c r="I12" s="20"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14" t="e">
+      <c r="L12" s="20"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="13"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
@@ -1809,60 +1875,61 @@
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
-      <c r="W12" s="14" t="e">
+      <c r="W12" s="13"/>
+      <c r="X12" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X12" s="24" t="e">
+      <c r="Y12" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="20"/>
+      <c r="Z12" s="26"/>
       <c r="AA12" s="20"/>
-      <c r="AB12" s="13"/>
+      <c r="AB12" s="20"/>
       <c r="AC12" s="13"/>
-      <c r="AD12" s="14" t="e">
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE12" s="24" t="e">
+      <c r="AF12" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF12" s="4"/>
-    </row>
-    <row r="13" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG12" s="4"/>
+    </row>
+    <row r="13" spans="1:40" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="1"/>
+      <c r="D13" s="7">
         <v>45216</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="14" t="e">
+      <c r="G13" s="13"/>
+      <c r="H13" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14" t="e">
+      <c r="I13" s="20"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14" t="e">
+      <c r="L13" s="20"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N13" s="20"/>
-      <c r="O13" s="13"/>
+      <c r="O13" s="20"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
@@ -1870,127 +1937,155 @@
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
-      <c r="W13" s="14" t="e">
+      <c r="W13" s="13"/>
+      <c r="X13" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X13" s="24" t="e">
+      <c r="Y13" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="20"/>
+      <c r="Z13" s="26"/>
       <c r="AA13" s="20"/>
-      <c r="AB13" s="13"/>
+      <c r="AB13" s="20"/>
       <c r="AC13" s="13"/>
-      <c r="AD13" s="14" t="e">
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE13" s="24" t="e">
+      <c r="AF13" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF13" s="4"/>
-    </row>
-    <row r="14" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG13" s="4"/>
+    </row>
+    <row r="14" spans="1:40" ht="14.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="7">
         <v>45015</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14" t="e">
+      <c r="E14" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="13">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="13">
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="14">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14" t="e">
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="I14" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="J14" s="13">
+        <v>3</v>
+      </c>
+      <c r="K14" s="14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14" t="e">
+        <v>3.3</v>
+      </c>
+      <c r="L14" s="20">
+        <v>0.62509999999999999</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="14">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13">
+        <v>2.5004</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13">
         <f xml:space="preserve"> AVERAGE(32.9, 34.4, 37.33, 48.63, 73.99, 49.73, 54.8, 34, 50.8, 92, 90.4, 42, 37.67, 34.8, 56, 69.66, 62.8, 29.2, 74.6, 53.57, 65.5, 86, 39.2, 51.6, 77.9, 41.74, 54.32, 69.3, 64.1)%</f>
         <v>0.5548068965517241</v>
       </c>
-      <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
-      <c r="U14" s="13">
+      <c r="U14" s="13"/>
+      <c r="V14" s="13">
         <f>AVERAGE(62.51, 62.47, 39.18, 61.22, 60.63)%</f>
         <v>0.57201999999999997</v>
       </c>
-      <c r="V14" s="13"/>
-      <c r="W14" s="14">
+      <c r="W14" s="13"/>
+      <c r="X14" s="14">
         <f t="shared" si="4"/>
         <v>2.2536537931034482</v>
       </c>
-      <c r="X14" s="24" t="e">
+      <c r="Y14" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="14" t="e">
+        <v>2.9697747356321837</v>
+      </c>
+      <c r="Z14" s="26">
+        <f>AVERAGE(4.5, 4, 4.8,4.7, 4.9)/5*4</f>
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="AA14" s="20">
+        <f>0.95*4</f>
+        <v>3.8</v>
+      </c>
+      <c r="AB14" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="AC14" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="AD14" s="13">
+        <v>3.75</v>
+      </c>
+      <c r="AE14" s="14">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE14" s="24" t="e">
+        <v>3.65</v>
+      </c>
+      <c r="AF14" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF14" s="4"/>
-    </row>
-    <row r="15" spans="1:39" ht="14.25" customHeight="1">
+        <v>3.6945000000000001</v>
+      </c>
+      <c r="AG14" s="4"/>
+    </row>
+    <row r="15" spans="1:40" ht="14.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="1"/>
+      <c r="D15" s="7">
         <v>45273</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="14" t="e">
+      <c r="G15" s="13"/>
+      <c r="H15" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14" t="e">
+      <c r="I15" s="20"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14" t="e">
+      <c r="L15" s="20"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="13"/>
+      <c r="O15" s="20"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
@@ -1998,60 +2093,61 @@
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
       <c r="V15" s="13"/>
-      <c r="W15" s="14" t="e">
+      <c r="W15" s="13"/>
+      <c r="X15" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X15" s="24" t="e">
+      <c r="Y15" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y15" s="27"/>
-      <c r="Z15" s="20"/>
+      <c r="Z15" s="26"/>
       <c r="AA15" s="20"/>
-      <c r="AB15" s="13"/>
+      <c r="AB15" s="20"/>
       <c r="AC15" s="13"/>
-      <c r="AD15" s="14" t="e">
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE15" s="24" t="e">
+      <c r="AF15" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF15" s="4"/>
-    </row>
-    <row r="16" spans="1:39" ht="14.25" customHeight="1">
+      <c r="AG15" s="4"/>
+    </row>
+    <row r="16" spans="1:40" ht="14.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="1"/>
+      <c r="D16" s="7">
         <v>45411</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="14" t="e">
+      <c r="G16" s="13"/>
+      <c r="H16" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14" t="e">
+      <c r="I16" s="20"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14" t="e">
+      <c r="L16" s="20"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="14" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="13"/>
+      <c r="O16" s="20"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
@@ -2059,60 +2155,80 @@
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
-      <c r="W16" s="14" t="e">
+      <c r="W16" s="13"/>
+      <c r="X16" s="14" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X16" s="24" t="e">
+      <c r="Y16" s="23" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="20"/>
+      <c r="Z16" s="26"/>
       <c r="AA16" s="20"/>
-      <c r="AB16" s="13"/>
+      <c r="AB16" s="20"/>
       <c r="AC16" s="13"/>
-      <c r="AD16" s="14" t="e">
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="14" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE16" s="24" t="e">
+      <c r="AF16" s="23" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF16" s="4"/>
-    </row>
-    <row r="17" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AG16" s="4"/>
+    </row>
+    <row r="17" spans="1:33" ht="14.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="7">
         <v>45126</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14" t="e">
+      <c r="E17" s="20">
+        <f>3-1</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="13">
+        <f>4.5-1</f>
+        <v>3.5</v>
+      </c>
+      <c r="G17" s="13">
+        <f>3.9-1</f>
+        <v>2.9</v>
+      </c>
+      <c r="H17" s="14">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14" t="e">
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="I17" s="20">
+        <f>4.3-1</f>
+        <v>3.3</v>
+      </c>
+      <c r="J17" s="13">
+        <f>4.2-1</f>
+        <v>3.2</v>
+      </c>
+      <c r="K17" s="14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14" t="e">
+        <v>3.25</v>
+      </c>
+      <c r="L17" s="20"/>
+      <c r="M17" s="13">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N17" s="14">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N17" s="20"/>
-      <c r="O17" s="13"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="O17" s="20"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
@@ -2120,32 +2236,49 @@
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
-      <c r="W17" s="14" t="e">
+      <c r="W17" s="13">
+        <v>0.53</v>
+      </c>
+      <c r="X17" s="14">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X17" s="24" t="e">
+        <v>2.12</v>
+      </c>
+      <c r="Y17" s="23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="14" t="e">
+        <v>2.7490000000000001</v>
+      </c>
+      <c r="Z17" s="26">
+        <f>3.5-1</f>
+        <v>2.5</v>
+      </c>
+      <c r="AA17" s="20">
+        <f>AVERAGE(3.4, 2)/5*4</f>
+        <v>2.16</v>
+      </c>
+      <c r="AB17" s="20">
+        <f>1.7-1</f>
+        <v>0.7</v>
+      </c>
+      <c r="AC17" s="13">
+        <f>1.5-1</f>
+        <v>0.5</v>
+      </c>
+      <c r="AD17" s="13">
+        <f>1.8-1</f>
+        <v>0.8</v>
+      </c>
+      <c r="AE17" s="14">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE17" s="24" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AF17" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF17" s="4"/>
-    </row>
-    <row r="18" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.9566666666666668</v>
+      </c>
+      <c r="AG17" s="4"/>
+    </row>
+    <row r="18" spans="1:33" ht="14.25" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -2165,19 +2298,19 @@
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="23"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
       <c r="AD18" s="4"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="4"/>
-    </row>
-    <row r="19" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="23"/>
+      <c r="AG18" s="4"/>
+    </row>
+    <row r="19" spans="1:33" ht="14.25" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -2197,19 +2330,19 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="23"/>
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
-      <c r="AE19" s="24"/>
-      <c r="AF19" s="4"/>
-    </row>
-    <row r="20" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="4"/>
+    </row>
+    <row r="20" spans="1:33" ht="14.25" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2229,19 +2362,19 @@
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="23"/>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
       <c r="AD20" s="4"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="4"/>
-    </row>
-    <row r="21" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="4"/>
+    </row>
+    <row r="21" spans="1:33" ht="14.25" customHeight="1">
       <c r="A21" s="3"/>
-      <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2261,19 +2394,19 @@
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="23"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
-      <c r="AE21" s="24"/>
-      <c r="AF21" s="4"/>
-    </row>
-    <row r="22" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="4"/>
+    </row>
+    <row r="22" spans="1:33" ht="14.25" customHeight="1">
       <c r="A22" s="3"/>
-      <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2293,19 +2426,19 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="23"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="4"/>
-    </row>
-    <row r="23" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="23"/>
+      <c r="AG22" s="4"/>
+    </row>
+    <row r="23" spans="1:33" ht="14.25" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2325,19 +2458,19 @@
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="23"/>
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="4"/>
-      <c r="AE23" s="24"/>
-      <c r="AF23" s="4"/>
-    </row>
-    <row r="24" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="4"/>
+    </row>
+    <row r="24" spans="1:33" ht="14.25" customHeight="1">
       <c r="A24" s="3"/>
-      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2357,24 +2490,24 @@
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="23"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="4"/>
-    </row>
-    <row r="25" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="4"/>
+    </row>
+    <row r="25" spans="1:33" ht="14.25" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="J25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -2384,17 +2517,17 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
-      <c r="X25" s="25"/>
-      <c r="AE25" s="25"/>
-    </row>
-    <row r="26" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W25" s="1"/>
+      <c r="Y25" s="24"/>
+      <c r="AF25" s="24"/>
+    </row>
+    <row r="26" spans="1:33" ht="14.25" customHeight="1">
       <c r="A26" s="3"/>
-      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="J26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -2404,17 +2537,17 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
-      <c r="X26" s="25"/>
-      <c r="AE26" s="25"/>
-    </row>
-    <row r="27" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W26" s="1"/>
+      <c r="Y26" s="24"/>
+      <c r="AF26" s="24"/>
+    </row>
+    <row r="27" spans="1:33" ht="14.25" customHeight="1">
       <c r="A27" s="3"/>
-      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="J27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -2424,17 +2557,17 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
-      <c r="X27" s="25"/>
-      <c r="AE27" s="25"/>
-    </row>
-    <row r="28" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W27" s="1"/>
+      <c r="Y27" s="24"/>
+      <c r="AF27" s="24"/>
+    </row>
+    <row r="28" spans="1:33" ht="14.25" customHeight="1">
       <c r="A28" s="3"/>
-      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="J28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -2444,17 +2577,17 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-      <c r="X28" s="25"/>
-      <c r="AE28" s="25"/>
-    </row>
-    <row r="29" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W28" s="1"/>
+      <c r="Y28" s="24"/>
+      <c r="AF28" s="24"/>
+    </row>
+    <row r="29" spans="1:33" ht="14.25" customHeight="1">
       <c r="A29" s="3"/>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="J29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -2464,17 +2597,17 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
-      <c r="X29" s="25"/>
-      <c r="AE29" s="25"/>
-    </row>
-    <row r="30" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W29" s="1"/>
+      <c r="Y29" s="24"/>
+      <c r="AF29" s="24"/>
+    </row>
+    <row r="30" spans="1:33" ht="14.25" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="J30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -2484,17 +2617,17 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
-      <c r="X30" s="25"/>
-      <c r="AE30" s="25"/>
-    </row>
-    <row r="31" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W30" s="1"/>
+      <c r="Y30" s="24"/>
+      <c r="AF30" s="24"/>
+    </row>
+    <row r="31" spans="1:33" ht="14.25" customHeight="1">
       <c r="A31" s="3"/>
-      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="F31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="J31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -2504,17 +2637,17 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
-      <c r="X31" s="25"/>
-      <c r="AE31" s="25"/>
-    </row>
-    <row r="32" spans="1:32" ht="14.25" customHeight="1">
+      <c r="W31" s="1"/>
+      <c r="Y31" s="24"/>
+      <c r="AF31" s="24"/>
+    </row>
+    <row r="32" spans="1:33" ht="14.25" customHeight="1">
       <c r="A32" s="3"/>
-      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="J32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -2524,17 +2657,17 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
-      <c r="X32" s="25"/>
-      <c r="AE32" s="25"/>
-    </row>
-    <row r="33" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W32" s="1"/>
+      <c r="Y32" s="24"/>
+      <c r="AF32" s="24"/>
+    </row>
+    <row r="33" spans="1:32" ht="14.25" customHeight="1">
       <c r="A33" s="3"/>
-      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="J33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -2544,17 +2677,17 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
-      <c r="X33" s="25"/>
-      <c r="AE33" s="25"/>
-    </row>
-    <row r="34" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W33" s="1"/>
+      <c r="Y33" s="24"/>
+      <c r="AF33" s="24"/>
+    </row>
+    <row r="34" spans="1:32" ht="14.25" customHeight="1">
       <c r="A34" s="3"/>
-      <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="J34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -2564,17 +2697,17 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
-      <c r="X34" s="25"/>
-      <c r="AE34" s="25"/>
-    </row>
-    <row r="35" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W34" s="1"/>
+      <c r="Y34" s="24"/>
+      <c r="AF34" s="24"/>
+    </row>
+    <row r="35" spans="1:32" ht="14.25" customHeight="1">
       <c r="A35" s="3"/>
-      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="M35" s="1"/>
+      <c r="J35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -2584,17 +2717,17 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
-      <c r="X35" s="25"/>
-      <c r="AE35" s="25"/>
-    </row>
-    <row r="36" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W35" s="1"/>
+      <c r="Y35" s="24"/>
+      <c r="AF35" s="24"/>
+    </row>
+    <row r="36" spans="1:32" ht="14.25" customHeight="1">
       <c r="A36" s="3"/>
-      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="J36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -2604,17 +2737,17 @@
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
-      <c r="X36" s="25"/>
-      <c r="AE36" s="25"/>
-    </row>
-    <row r="37" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W36" s="1"/>
+      <c r="Y36" s="24"/>
+      <c r="AF36" s="24"/>
+    </row>
+    <row r="37" spans="1:32" ht="14.25" customHeight="1">
       <c r="A37" s="3"/>
-      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="J37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -2624,17 +2757,17 @@
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
-      <c r="X37" s="25"/>
-      <c r="AE37" s="25"/>
-    </row>
-    <row r="38" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W37" s="1"/>
+      <c r="Y37" s="24"/>
+      <c r="AF37" s="24"/>
+    </row>
+    <row r="38" spans="1:32" ht="14.25" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="J38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -2644,17 +2777,17 @@
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
-      <c r="X38" s="25"/>
-      <c r="AE38" s="25"/>
-    </row>
-    <row r="39" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W38" s="1"/>
+      <c r="Y38" s="24"/>
+      <c r="AF38" s="24"/>
+    </row>
+    <row r="39" spans="1:32" ht="14.25" customHeight="1">
       <c r="A39" s="3"/>
-      <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="F39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="M39" s="1"/>
+      <c r="J39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -2664,17 +2797,17 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
-      <c r="X39" s="25"/>
-      <c r="AE39" s="25"/>
-    </row>
-    <row r="40" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W39" s="1"/>
+      <c r="Y39" s="24"/>
+      <c r="AF39" s="24"/>
+    </row>
+    <row r="40" spans="1:32" ht="14.25" customHeight="1">
       <c r="A40" s="3"/>
-      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="F40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="M40" s="1"/>
+      <c r="J40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -2684,17 +2817,17 @@
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
-      <c r="X40" s="25"/>
-      <c r="AE40" s="25"/>
-    </row>
-    <row r="41" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W40" s="1"/>
+      <c r="Y40" s="24"/>
+      <c r="AF40" s="24"/>
+    </row>
+    <row r="41" spans="1:32" ht="14.25" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="F41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="M41" s="1"/>
+      <c r="J41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2704,17 +2837,17 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
-      <c r="X41" s="25"/>
-      <c r="AE41" s="25"/>
-    </row>
-    <row r="42" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W41" s="1"/>
+      <c r="Y41" s="24"/>
+      <c r="AF41" s="24"/>
+    </row>
+    <row r="42" spans="1:32" ht="14.25" customHeight="1">
       <c r="A42" s="3"/>
-      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="F42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="M42" s="1"/>
+      <c r="J42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -2724,17 +2857,17 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
-      <c r="X42" s="25"/>
-      <c r="AE42" s="25"/>
-    </row>
-    <row r="43" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W42" s="1"/>
+      <c r="Y42" s="24"/>
+      <c r="AF42" s="24"/>
+    </row>
+    <row r="43" spans="1:32" ht="14.25" customHeight="1">
       <c r="A43" s="3"/>
-      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="F43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="M43" s="1"/>
+      <c r="J43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -2744,17 +2877,17 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
-      <c r="X43" s="25"/>
-      <c r="AE43" s="25"/>
-    </row>
-    <row r="44" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W43" s="1"/>
+      <c r="Y43" s="24"/>
+      <c r="AF43" s="24"/>
+    </row>
+    <row r="44" spans="1:32" ht="14.25" customHeight="1">
       <c r="A44" s="3"/>
-      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="F44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="M44" s="1"/>
+      <c r="J44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -2764,17 +2897,17 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
-      <c r="X44" s="25"/>
-      <c r="AE44" s="25"/>
-    </row>
-    <row r="45" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W44" s="1"/>
+      <c r="Y44" s="24"/>
+      <c r="AF44" s="24"/>
+    </row>
+    <row r="45" spans="1:32" ht="14.25" customHeight="1">
       <c r="A45" s="3"/>
-      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="F45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="M45" s="1"/>
+      <c r="J45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -2784,17 +2917,17 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
-      <c r="X45" s="25"/>
-      <c r="AE45" s="25"/>
-    </row>
-    <row r="46" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W45" s="1"/>
+      <c r="Y45" s="24"/>
+      <c r="AF45" s="24"/>
+    </row>
+    <row r="46" spans="1:32" ht="14.25" customHeight="1">
       <c r="A46" s="3"/>
-      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="F46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="M46" s="1"/>
+      <c r="J46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -2804,17 +2937,17 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
-      <c r="X46" s="25"/>
-      <c r="AE46" s="25"/>
-    </row>
-    <row r="47" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W46" s="1"/>
+      <c r="Y46" s="24"/>
+      <c r="AF46" s="24"/>
+    </row>
+    <row r="47" spans="1:32" ht="14.25" customHeight="1">
       <c r="A47" s="3"/>
-      <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="F47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="M47" s="1"/>
+      <c r="J47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -2824,17 +2957,17 @@
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
-      <c r="X47" s="25"/>
-      <c r="AE47" s="25"/>
-    </row>
-    <row r="48" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W47" s="1"/>
+      <c r="Y47" s="24"/>
+      <c r="AF47" s="24"/>
+    </row>
+    <row r="48" spans="1:32" ht="14.25" customHeight="1">
       <c r="A48" s="3"/>
-      <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="F48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="M48" s="1"/>
+      <c r="J48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -2844,17 +2977,17 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
-      <c r="X48" s="25"/>
-      <c r="AE48" s="25"/>
-    </row>
-    <row r="49" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W48" s="1"/>
+      <c r="Y48" s="24"/>
+      <c r="AF48" s="24"/>
+    </row>
+    <row r="49" spans="1:32" ht="14.25" customHeight="1">
       <c r="A49" s="3"/>
-      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="F49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="M49" s="1"/>
+      <c r="J49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -2864,17 +2997,17 @@
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
-      <c r="X49" s="25"/>
-      <c r="AE49" s="25"/>
-    </row>
-    <row r="50" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W49" s="1"/>
+      <c r="Y49" s="24"/>
+      <c r="AF49" s="24"/>
+    </row>
+    <row r="50" spans="1:32" ht="14.25" customHeight="1">
       <c r="A50" s="3"/>
-      <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="F50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="M50" s="1"/>
+      <c r="J50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
@@ -2884,17 +3017,17 @@
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
-      <c r="X50" s="25"/>
-      <c r="AE50" s="25"/>
-    </row>
-    <row r="51" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W50" s="1"/>
+      <c r="Y50" s="24"/>
+      <c r="AF50" s="24"/>
+    </row>
+    <row r="51" spans="1:32" ht="14.25" customHeight="1">
       <c r="A51" s="3"/>
-      <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="F51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="M51" s="1"/>
+      <c r="J51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
@@ -2904,17 +3037,17 @@
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
-      <c r="X51" s="25"/>
-      <c r="AE51" s="25"/>
-    </row>
-    <row r="52" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W51" s="1"/>
+      <c r="Y51" s="24"/>
+      <c r="AF51" s="24"/>
+    </row>
+    <row r="52" spans="1:32" ht="14.25" customHeight="1">
       <c r="A52" s="3"/>
-      <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="F52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="M52" s="1"/>
+      <c r="J52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -2924,17 +3057,17 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
-      <c r="X52" s="25"/>
-      <c r="AE52" s="25"/>
-    </row>
-    <row r="53" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W52" s="1"/>
+      <c r="Y52" s="24"/>
+      <c r="AF52" s="24"/>
+    </row>
+    <row r="53" spans="1:32" ht="14.25" customHeight="1">
       <c r="A53" s="3"/>
-      <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="M53" s="1"/>
+      <c r="J53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -2944,17 +3077,17 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
-      <c r="X53" s="25"/>
-      <c r="AE53" s="25"/>
-    </row>
-    <row r="54" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W53" s="1"/>
+      <c r="Y53" s="24"/>
+      <c r="AF53" s="24"/>
+    </row>
+    <row r="54" spans="1:32" ht="14.25" customHeight="1">
       <c r="A54" s="3"/>
-      <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="F54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-      <c r="M54" s="1"/>
+      <c r="J54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -2964,17 +3097,17 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
-      <c r="X54" s="25"/>
-      <c r="AE54" s="25"/>
-    </row>
-    <row r="55" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W54" s="1"/>
+      <c r="Y54" s="24"/>
+      <c r="AF54" s="24"/>
+    </row>
+    <row r="55" spans="1:32" ht="14.25" customHeight="1">
       <c r="A55" s="3"/>
-      <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="F55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-      <c r="M55" s="1"/>
+      <c r="J55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
@@ -2984,17 +3117,17 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
-      <c r="X55" s="25"/>
-      <c r="AE55" s="25"/>
-    </row>
-    <row r="56" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W55" s="1"/>
+      <c r="Y55" s="24"/>
+      <c r="AF55" s="24"/>
+    </row>
+    <row r="56" spans="1:32" ht="14.25" customHeight="1">
       <c r="A56" s="3"/>
-      <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="F56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-      <c r="M56" s="1"/>
+      <c r="J56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -3004,17 +3137,17 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
-      <c r="X56" s="25"/>
-      <c r="AE56" s="25"/>
-    </row>
-    <row r="57" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W56" s="1"/>
+      <c r="Y56" s="24"/>
+      <c r="AF56" s="24"/>
+    </row>
+    <row r="57" spans="1:32" ht="14.25" customHeight="1">
       <c r="A57" s="3"/>
-      <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="F57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="M57" s="1"/>
+      <c r="J57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
@@ -3024,17 +3157,17 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
-      <c r="X57" s="25"/>
-      <c r="AE57" s="25"/>
-    </row>
-    <row r="58" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W57" s="1"/>
+      <c r="Y57" s="24"/>
+      <c r="AF57" s="24"/>
+    </row>
+    <row r="58" spans="1:32" ht="14.25" customHeight="1">
       <c r="A58" s="3"/>
-      <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="F58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-      <c r="M58" s="1"/>
+      <c r="J58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
@@ -3044,17 +3177,17 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
-      <c r="X58" s="25"/>
-      <c r="AE58" s="25"/>
-    </row>
-    <row r="59" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W58" s="1"/>
+      <c r="Y58" s="24"/>
+      <c r="AF58" s="24"/>
+    </row>
+    <row r="59" spans="1:32" ht="14.25" customHeight="1">
       <c r="A59" s="3"/>
-      <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="F59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-      <c r="M59" s="1"/>
+      <c r="J59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
@@ -3064,17 +3197,17 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
-      <c r="X59" s="25"/>
-      <c r="AE59" s="25"/>
-    </row>
-    <row r="60" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W59" s="1"/>
+      <c r="Y59" s="24"/>
+      <c r="AF59" s="24"/>
+    </row>
+    <row r="60" spans="1:32" ht="14.25" customHeight="1">
       <c r="A60" s="3"/>
-      <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="G60" s="1"/>
+      <c r="F60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
-      <c r="M60" s="1"/>
+      <c r="J60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
@@ -3084,17 +3217,17 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
-      <c r="X60" s="25"/>
-      <c r="AE60" s="25"/>
-    </row>
-    <row r="61" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W60" s="1"/>
+      <c r="Y60" s="24"/>
+      <c r="AF60" s="24"/>
+    </row>
+    <row r="61" spans="1:32" ht="14.25" customHeight="1">
       <c r="A61" s="3"/>
-      <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="F61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-      <c r="M61" s="1"/>
+      <c r="J61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
@@ -3104,17 +3237,17 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
-      <c r="X61" s="25"/>
-      <c r="AE61" s="25"/>
-    </row>
-    <row r="62" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W61" s="1"/>
+      <c r="Y61" s="24"/>
+      <c r="AF61" s="24"/>
+    </row>
+    <row r="62" spans="1:32" ht="14.25" customHeight="1">
       <c r="A62" s="3"/>
-      <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="G62" s="1"/>
+      <c r="F62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
-      <c r="M62" s="1"/>
+      <c r="J62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -3124,17 +3257,17 @@
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
-      <c r="X62" s="25"/>
-      <c r="AE62" s="25"/>
-    </row>
-    <row r="63" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W62" s="1"/>
+      <c r="Y62" s="24"/>
+      <c r="AF62" s="24"/>
+    </row>
+    <row r="63" spans="1:32" ht="14.25" customHeight="1">
       <c r="A63" s="3"/>
-      <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="F63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-      <c r="M63" s="1"/>
+      <c r="J63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
@@ -3144,17 +3277,17 @@
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
-      <c r="X63" s="25"/>
-      <c r="AE63" s="25"/>
-    </row>
-    <row r="64" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W63" s="1"/>
+      <c r="Y63" s="24"/>
+      <c r="AF63" s="24"/>
+    </row>
+    <row r="64" spans="1:32" ht="14.25" customHeight="1">
       <c r="A64" s="3"/>
-      <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="F64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-      <c r="M64" s="1"/>
+      <c r="J64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -3164,17 +3297,17 @@
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
       <c r="V64" s="1"/>
-      <c r="X64" s="25"/>
-      <c r="AE64" s="25"/>
-    </row>
-    <row r="65" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W64" s="1"/>
+      <c r="Y64" s="24"/>
+      <c r="AF64" s="24"/>
+    </row>
+    <row r="65" spans="1:32" ht="14.25" customHeight="1">
       <c r="A65" s="3"/>
-      <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="G65" s="1"/>
+      <c r="F65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-      <c r="M65" s="1"/>
+      <c r="J65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -3184,17 +3317,17 @@
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
-      <c r="X65" s="25"/>
-      <c r="AE65" s="25"/>
-    </row>
-    <row r="66" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W65" s="1"/>
+      <c r="Y65" s="24"/>
+      <c r="AF65" s="24"/>
+    </row>
+    <row r="66" spans="1:32" ht="14.25" customHeight="1">
       <c r="A66" s="3"/>
-      <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="G66" s="1"/>
+      <c r="F66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-      <c r="M66" s="1"/>
+      <c r="J66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
@@ -3204,17 +3337,17 @@
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
-      <c r="X66" s="25"/>
-      <c r="AE66" s="25"/>
-    </row>
-    <row r="67" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W66" s="1"/>
+      <c r="Y66" s="24"/>
+      <c r="AF66" s="24"/>
+    </row>
+    <row r="67" spans="1:32" ht="14.25" customHeight="1">
       <c r="A67" s="3"/>
-      <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="G67" s="1"/>
+      <c r="F67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
-      <c r="M67" s="1"/>
+      <c r="J67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
@@ -3224,17 +3357,17 @@
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
-      <c r="X67" s="25"/>
-      <c r="AE67" s="25"/>
-    </row>
-    <row r="68" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W67" s="1"/>
+      <c r="Y67" s="24"/>
+      <c r="AF67" s="24"/>
+    </row>
+    <row r="68" spans="1:32" ht="14.25" customHeight="1">
       <c r="A68" s="3"/>
-      <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="G68" s="1"/>
+      <c r="F68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
-      <c r="M68" s="1"/>
+      <c r="J68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
@@ -3244,17 +3377,17 @@
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
-      <c r="X68" s="25"/>
-      <c r="AE68" s="25"/>
-    </row>
-    <row r="69" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W68" s="1"/>
+      <c r="Y68" s="24"/>
+      <c r="AF68" s="24"/>
+    </row>
+    <row r="69" spans="1:32" ht="14.25" customHeight="1">
       <c r="A69" s="3"/>
-      <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="F69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-      <c r="M69" s="1"/>
+      <c r="J69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
@@ -3264,17 +3397,17 @@
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
-      <c r="X69" s="25"/>
-      <c r="AE69" s="25"/>
-    </row>
-    <row r="70" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W69" s="1"/>
+      <c r="Y69" s="24"/>
+      <c r="AF69" s="24"/>
+    </row>
+    <row r="70" spans="1:32" ht="14.25" customHeight="1">
       <c r="A70" s="3"/>
-      <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="G70" s="1"/>
+      <c r="F70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-      <c r="M70" s="1"/>
+      <c r="J70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -3284,17 +3417,17 @@
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
-      <c r="X70" s="25"/>
-      <c r="AE70" s="25"/>
-    </row>
-    <row r="71" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W70" s="1"/>
+      <c r="Y70" s="24"/>
+      <c r="AF70" s="24"/>
+    </row>
+    <row r="71" spans="1:32" ht="14.25" customHeight="1">
       <c r="A71" s="3"/>
-      <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="G71" s="1"/>
+      <c r="F71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-      <c r="M71" s="1"/>
+      <c r="J71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -3304,17 +3437,17 @@
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
-      <c r="X71" s="25"/>
-      <c r="AE71" s="25"/>
-    </row>
-    <row r="72" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W71" s="1"/>
+      <c r="Y71" s="24"/>
+      <c r="AF71" s="24"/>
+    </row>
+    <row r="72" spans="1:32" ht="14.25" customHeight="1">
       <c r="A72" s="3"/>
-      <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="G72" s="1"/>
+      <c r="F72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="M72" s="1"/>
+      <c r="J72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -3324,17 +3457,17 @@
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
-      <c r="X72" s="25"/>
-      <c r="AE72" s="25"/>
-    </row>
-    <row r="73" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W72" s="1"/>
+      <c r="Y72" s="24"/>
+      <c r="AF72" s="24"/>
+    </row>
+    <row r="73" spans="1:32" ht="14.25" customHeight="1">
       <c r="A73" s="3"/>
-      <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="F73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="M73" s="1"/>
+      <c r="J73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -3344,17 +3477,17 @@
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
-      <c r="X73" s="25"/>
-      <c r="AE73" s="25"/>
-    </row>
-    <row r="74" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W73" s="1"/>
+      <c r="Y73" s="24"/>
+      <c r="AF73" s="24"/>
+    </row>
+    <row r="74" spans="1:32" ht="14.25" customHeight="1">
       <c r="A74" s="3"/>
-      <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="F74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
-      <c r="M74" s="1"/>
+      <c r="J74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
@@ -3364,17 +3497,17 @@
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
-      <c r="X74" s="25"/>
-      <c r="AE74" s="25"/>
-    </row>
-    <row r="75" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W74" s="1"/>
+      <c r="Y74" s="24"/>
+      <c r="AF74" s="24"/>
+    </row>
+    <row r="75" spans="1:32" ht="14.25" customHeight="1">
       <c r="A75" s="3"/>
-      <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="F75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
-      <c r="M75" s="1"/>
+      <c r="J75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
@@ -3384,17 +3517,17 @@
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
-      <c r="X75" s="25"/>
-      <c r="AE75" s="25"/>
-    </row>
-    <row r="76" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W75" s="1"/>
+      <c r="Y75" s="24"/>
+      <c r="AF75" s="24"/>
+    </row>
+    <row r="76" spans="1:32" ht="14.25" customHeight="1">
       <c r="A76" s="3"/>
-      <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="F76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
-      <c r="M76" s="1"/>
+      <c r="J76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
@@ -3404,17 +3537,17 @@
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
-      <c r="X76" s="25"/>
-      <c r="AE76" s="25"/>
-    </row>
-    <row r="77" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W76" s="1"/>
+      <c r="Y76" s="24"/>
+      <c r="AF76" s="24"/>
+    </row>
+    <row r="77" spans="1:32" ht="14.25" customHeight="1">
       <c r="A77" s="3"/>
-      <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="G77" s="1"/>
+      <c r="F77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
-      <c r="M77" s="1"/>
+      <c r="J77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
@@ -3424,17 +3557,17 @@
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
-      <c r="X77" s="25"/>
-      <c r="AE77" s="25"/>
-    </row>
-    <row r="78" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W77" s="1"/>
+      <c r="Y77" s="24"/>
+      <c r="AF77" s="24"/>
+    </row>
+    <row r="78" spans="1:32" ht="14.25" customHeight="1">
       <c r="A78" s="3"/>
-      <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="G78" s="1"/>
+      <c r="F78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
-      <c r="M78" s="1"/>
+      <c r="J78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
@@ -3444,17 +3577,17 @@
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
       <c r="V78" s="1"/>
-      <c r="X78" s="25"/>
-      <c r="AE78" s="25"/>
-    </row>
-    <row r="79" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W78" s="1"/>
+      <c r="Y78" s="24"/>
+      <c r="AF78" s="24"/>
+    </row>
+    <row r="79" spans="1:32" ht="14.25" customHeight="1">
       <c r="A79" s="3"/>
-      <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="G79" s="1"/>
+      <c r="F79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
-      <c r="M79" s="1"/>
+      <c r="J79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
@@ -3464,17 +3597,17 @@
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
       <c r="V79" s="1"/>
-      <c r="X79" s="25"/>
-      <c r="AE79" s="25"/>
-    </row>
-    <row r="80" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W79" s="1"/>
+      <c r="Y79" s="24"/>
+      <c r="AF79" s="24"/>
+    </row>
+    <row r="80" spans="1:32" ht="14.25" customHeight="1">
       <c r="A80" s="3"/>
-      <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="G80" s="1"/>
+      <c r="F80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
-      <c r="M80" s="1"/>
+      <c r="J80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
@@ -3484,17 +3617,17 @@
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
-      <c r="X80" s="25"/>
-      <c r="AE80" s="25"/>
-    </row>
-    <row r="81" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W80" s="1"/>
+      <c r="Y80" s="24"/>
+      <c r="AF80" s="24"/>
+    </row>
+    <row r="81" spans="1:32" ht="14.25" customHeight="1">
       <c r="A81" s="3"/>
-      <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="F81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
-      <c r="M81" s="1"/>
+      <c r="J81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
@@ -3504,17 +3637,17 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
-      <c r="X81" s="25"/>
-      <c r="AE81" s="25"/>
-    </row>
-    <row r="82" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W81" s="1"/>
+      <c r="Y81" s="24"/>
+      <c r="AF81" s="24"/>
+    </row>
+    <row r="82" spans="1:32" ht="14.25" customHeight="1">
       <c r="A82" s="3"/>
-      <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="F82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
-      <c r="M82" s="1"/>
+      <c r="J82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -3524,17 +3657,17 @@
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
-      <c r="X82" s="25"/>
-      <c r="AE82" s="25"/>
-    </row>
-    <row r="83" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W82" s="1"/>
+      <c r="Y82" s="24"/>
+      <c r="AF82" s="24"/>
+    </row>
+    <row r="83" spans="1:32" ht="14.25" customHeight="1">
       <c r="A83" s="3"/>
-      <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="F83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
-      <c r="M83" s="1"/>
+      <c r="J83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
@@ -3544,17 +3677,17 @@
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
       <c r="V83" s="1"/>
-      <c r="X83" s="25"/>
-      <c r="AE83" s="25"/>
-    </row>
-    <row r="84" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W83" s="1"/>
+      <c r="Y83" s="24"/>
+      <c r="AF83" s="24"/>
+    </row>
+    <row r="84" spans="1:32" ht="14.25" customHeight="1">
       <c r="A84" s="3"/>
-      <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="F84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
-      <c r="M84" s="1"/>
+      <c r="J84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
@@ -3564,17 +3697,17 @@
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
-      <c r="X84" s="25"/>
-      <c r="AE84" s="25"/>
-    </row>
-    <row r="85" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W84" s="1"/>
+      <c r="Y84" s="24"/>
+      <c r="AF84" s="24"/>
+    </row>
+    <row r="85" spans="1:32" ht="14.25" customHeight="1">
       <c r="A85" s="3"/>
-      <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="G85" s="1"/>
+      <c r="F85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
-      <c r="M85" s="1"/>
+      <c r="J85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -3584,17 +3717,17 @@
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
       <c r="V85" s="1"/>
-      <c r="X85" s="25"/>
-      <c r="AE85" s="25"/>
-    </row>
-    <row r="86" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W85" s="1"/>
+      <c r="Y85" s="24"/>
+      <c r="AF85" s="24"/>
+    </row>
+    <row r="86" spans="1:32" ht="14.25" customHeight="1">
       <c r="A86" s="3"/>
-      <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="G86" s="1"/>
+      <c r="F86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
-      <c r="M86" s="1"/>
+      <c r="J86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
@@ -3604,17 +3737,17 @@
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
-      <c r="X86" s="25"/>
-      <c r="AE86" s="25"/>
-    </row>
-    <row r="87" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W86" s="1"/>
+      <c r="Y86" s="24"/>
+      <c r="AF86" s="24"/>
+    </row>
+    <row r="87" spans="1:32" ht="14.25" customHeight="1">
       <c r="A87" s="3"/>
-      <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-      <c r="G87" s="1"/>
+      <c r="F87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
-      <c r="M87" s="1"/>
+      <c r="J87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
@@ -3624,17 +3757,17 @@
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
-      <c r="X87" s="25"/>
-      <c r="AE87" s="25"/>
-    </row>
-    <row r="88" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W87" s="1"/>
+      <c r="Y87" s="24"/>
+      <c r="AF87" s="24"/>
+    </row>
+    <row r="88" spans="1:32" ht="14.25" customHeight="1">
       <c r="A88" s="3"/>
-      <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="G88" s="1"/>
+      <c r="F88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
-      <c r="M88" s="1"/>
+      <c r="J88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
@@ -3644,17 +3777,17 @@
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
-      <c r="X88" s="25"/>
-      <c r="AE88" s="25"/>
-    </row>
-    <row r="89" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W88" s="1"/>
+      <c r="Y88" s="24"/>
+      <c r="AF88" s="24"/>
+    </row>
+    <row r="89" spans="1:32" ht="14.25" customHeight="1">
       <c r="A89" s="3"/>
-      <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-      <c r="G89" s="1"/>
+      <c r="F89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
-      <c r="M89" s="1"/>
+      <c r="J89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
@@ -3664,17 +3797,17 @@
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
       <c r="V89" s="1"/>
-      <c r="X89" s="25"/>
-      <c r="AE89" s="25"/>
-    </row>
-    <row r="90" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W89" s="1"/>
+      <c r="Y89" s="24"/>
+      <c r="AF89" s="24"/>
+    </row>
+    <row r="90" spans="1:32" ht="14.25" customHeight="1">
       <c r="A90" s="3"/>
-      <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-      <c r="G90" s="1"/>
+      <c r="F90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
-      <c r="M90" s="1"/>
+      <c r="J90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
@@ -3684,17 +3817,17 @@
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
       <c r="V90" s="1"/>
-      <c r="X90" s="25"/>
-      <c r="AE90" s="25"/>
-    </row>
-    <row r="91" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W90" s="1"/>
+      <c r="Y90" s="24"/>
+      <c r="AF90" s="24"/>
+    </row>
+    <row r="91" spans="1:32" ht="14.25" customHeight="1">
       <c r="A91" s="3"/>
-      <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="G91" s="1"/>
+      <c r="F91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
-      <c r="M91" s="1"/>
+      <c r="J91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
@@ -3704,17 +3837,17 @@
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
       <c r="V91" s="1"/>
-      <c r="X91" s="25"/>
-      <c r="AE91" s="25"/>
-    </row>
-    <row r="92" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W91" s="1"/>
+      <c r="Y91" s="24"/>
+      <c r="AF91" s="24"/>
+    </row>
+    <row r="92" spans="1:32" ht="14.25" customHeight="1">
       <c r="A92" s="3"/>
-      <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="G92" s="1"/>
+      <c r="F92" s="1"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
-      <c r="M92" s="1"/>
+      <c r="J92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
@@ -3724,17 +3857,17 @@
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
       <c r="V92" s="1"/>
-      <c r="X92" s="25"/>
-      <c r="AE92" s="25"/>
-    </row>
-    <row r="93" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W92" s="1"/>
+      <c r="Y92" s="24"/>
+      <c r="AF92" s="24"/>
+    </row>
+    <row r="93" spans="1:32" ht="14.25" customHeight="1">
       <c r="A93" s="3"/>
-      <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="G93" s="1"/>
+      <c r="F93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
-      <c r="M93" s="1"/>
+      <c r="J93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
@@ -3744,17 +3877,17 @@
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
       <c r="V93" s="1"/>
-      <c r="X93" s="25"/>
-      <c r="AE93" s="25"/>
-    </row>
-    <row r="94" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W93" s="1"/>
+      <c r="Y93" s="24"/>
+      <c r="AF93" s="24"/>
+    </row>
+    <row r="94" spans="1:32" ht="14.25" customHeight="1">
       <c r="A94" s="3"/>
-      <c r="D94" s="1"/>
       <c r="E94" s="1"/>
-      <c r="G94" s="1"/>
+      <c r="F94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-      <c r="M94" s="1"/>
+      <c r="J94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
@@ -3764,17 +3897,17 @@
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
-      <c r="X94" s="25"/>
-      <c r="AE94" s="25"/>
-    </row>
-    <row r="95" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W94" s="1"/>
+      <c r="Y94" s="24"/>
+      <c r="AF94" s="24"/>
+    </row>
+    <row r="95" spans="1:32" ht="14.25" customHeight="1">
       <c r="A95" s="3"/>
-      <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-      <c r="G95" s="1"/>
+      <c r="F95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
-      <c r="M95" s="1"/>
+      <c r="J95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
@@ -3784,17 +3917,17 @@
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
-      <c r="X95" s="25"/>
-      <c r="AE95" s="25"/>
-    </row>
-    <row r="96" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W95" s="1"/>
+      <c r="Y95" s="24"/>
+      <c r="AF95" s="24"/>
+    </row>
+    <row r="96" spans="1:32" ht="14.25" customHeight="1">
       <c r="A96" s="3"/>
-      <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-      <c r="G96" s="1"/>
+      <c r="F96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
-      <c r="M96" s="1"/>
+      <c r="J96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
@@ -3804,17 +3937,17 @@
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
       <c r="V96" s="1"/>
-      <c r="X96" s="25"/>
-      <c r="AE96" s="25"/>
-    </row>
-    <row r="97" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W96" s="1"/>
+      <c r="Y96" s="24"/>
+      <c r="AF96" s="24"/>
+    </row>
+    <row r="97" spans="1:32" ht="14.25" customHeight="1">
       <c r="A97" s="3"/>
-      <c r="D97" s="1"/>
       <c r="E97" s="1"/>
-      <c r="G97" s="1"/>
+      <c r="F97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
-      <c r="M97" s="1"/>
+      <c r="J97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
@@ -3824,17 +3957,17 @@
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
       <c r="V97" s="1"/>
-      <c r="X97" s="25"/>
-      <c r="AE97" s="25"/>
-    </row>
-    <row r="98" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W97" s="1"/>
+      <c r="Y97" s="24"/>
+      <c r="AF97" s="24"/>
+    </row>
+    <row r="98" spans="1:32" ht="14.25" customHeight="1">
       <c r="A98" s="3"/>
-      <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-      <c r="G98" s="1"/>
+      <c r="F98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
-      <c r="M98" s="1"/>
+      <c r="J98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
@@ -3844,17 +3977,17 @@
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
       <c r="V98" s="1"/>
-      <c r="X98" s="25"/>
-      <c r="AE98" s="25"/>
-    </row>
-    <row r="99" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W98" s="1"/>
+      <c r="Y98" s="24"/>
+      <c r="AF98" s="24"/>
+    </row>
+    <row r="99" spans="1:32" ht="14.25" customHeight="1">
       <c r="A99" s="3"/>
-      <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-      <c r="G99" s="1"/>
+      <c r="F99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
-      <c r="M99" s="1"/>
+      <c r="J99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
@@ -3864,17 +3997,17 @@
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
       <c r="V99" s="1"/>
-      <c r="X99" s="25"/>
-      <c r="AE99" s="25"/>
-    </row>
-    <row r="100" spans="1:31" ht="14.25" customHeight="1">
+      <c r="W99" s="1"/>
+      <c r="Y99" s="24"/>
+      <c r="AF99" s="24"/>
+    </row>
+    <row r="100" spans="1:32" ht="14.25" customHeight="1">
       <c r="A100" s="3"/>
-      <c r="D100" s="1"/>
       <c r="E100" s="1"/>
-      <c r="G100" s="1"/>
+      <c r="F100" s="1"/>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
-      <c r="M100" s="1"/>
+      <c r="J100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
@@ -3884,18 +4017,19 @@
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
       <c r="V100" s="1"/>
-      <c r="X100" s="25"/>
-      <c r="AE100" s="25"/>
+      <c r="W100" s="1"/>
+      <c r="Y100" s="24"/>
+      <c r="AF100" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:W2"/>
-    <mergeCell ref="D1:X1"/>
-    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:X2"/>
+    <mergeCell ref="E1:Y1"/>
+    <mergeCell ref="AB2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update LLM Matrix (6/6)
</commit_message>
<xml_diff>
--- a/data/LLM Matrix.xlsx
+++ b/data/LLM Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Business Rediness - &gt; x-axis</t>
   </si>
@@ -230,7 +230,24 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Specialised for Manufacturing, Research, Finance and </t>
+      <t xml:space="preserve">Specialised for Manufacturing, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, Finance and </t>
     </r>
     <r>
       <rPr>
@@ -286,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -361,11 +378,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -414,6 +444,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +517,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.3825271351575457</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -535,7 +568,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.2583333333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1030,14 +1063,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="3" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" customWidth="1"/>
     <col min="4" max="4" width="12.453125" style="5" customWidth="1"/>
     <col min="5" max="6" width="12.453125" customWidth="1"/>
     <col min="7" max="10" width="13.81640625" customWidth="1"/>
@@ -1118,6 +1152,7 @@
       <c r="W2" s="11"/>
       <c r="X2" s="12"/>
       <c r="Y2" s="21"/>
+      <c r="Z2" s="38"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="27" t="s">
         <v>28</v>
@@ -1290,7 +1325,7 @@
         <v>3.0406666666666666</v>
       </c>
       <c r="Y4" s="23">
-        <f t="shared" ref="Y4:Y17" si="2">0.4*H4+0.3*K4+0.15*N4+0.15*X4</f>
+        <f>0.4*H4+0.3*K4+0.15*N4+0.15*X4</f>
         <v>2.6909666666666663</v>
       </c>
       <c r="Z4" s="26">
@@ -1347,7 +1382,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="13"/>
       <c r="N5" s="14" t="e">
-        <f t="shared" ref="N5:N17" si="3">AVERAGE(L5:M5)*4</f>
+        <f t="shared" ref="N5:N17" si="2">AVERAGE(L5:M5)*4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O5" s="20"/>
@@ -1360,11 +1395,11 @@
       <c r="V5" s="13"/>
       <c r="W5" s="13"/>
       <c r="X5" s="14" t="e">
-        <f t="shared" ref="X5:X17" si="4">AVERAGE(O5,P5,Q5,R5,S5,T5,U5,V5,W5)*4</f>
+        <f t="shared" ref="X5:X17" si="3">AVERAGE(O5,P5,Q5,R5,S5,T5,U5,V5,W5)*4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Y5" s="23" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="Y4:Y17" si="4">0.4*H5+0.3*K5+0.15*N5+0.15*X5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Z5" s="26"/>
@@ -1416,7 +1451,7 @@
       <c r="L6" s="20"/>
       <c r="M6" s="13"/>
       <c r="N6" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O6" s="20"/>
@@ -1429,11 +1464,11 @@
       <c r="V6" s="13"/>
       <c r="W6" s="13"/>
       <c r="X6" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y6" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y6" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z6" s="26"/>
@@ -1500,7 +1535,7 @@
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.6566666666666667</v>
       </c>
       <c r="O7" s="20"/>
@@ -1521,11 +1556,11 @@
       <c r="V7" s="13"/>
       <c r="W7" s="13"/>
       <c r="X7" s="14">
+        <f t="shared" si="3"/>
+        <v>2.4291</v>
+      </c>
+      <c r="Y7" s="23">
         <f t="shared" si="4"/>
-        <v>2.4291</v>
-      </c>
-      <c r="Y7" s="23">
-        <f t="shared" si="2"/>
         <v>2.4211983333333329</v>
       </c>
       <c r="Z7" s="26">
@@ -1599,7 +1634,7 @@
         <v>0.63</v>
       </c>
       <c r="N8" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.52</v>
       </c>
       <c r="O8" s="20"/>
@@ -1614,11 +1649,11 @@
         <v>0.49998999999999999</v>
       </c>
       <c r="X8" s="14">
+        <f t="shared" si="3"/>
+        <v>1.99996</v>
+      </c>
+      <c r="Y8" s="23">
         <f t="shared" si="4"/>
-        <v>1.99996</v>
-      </c>
-      <c r="Y8" s="23">
-        <f t="shared" si="2"/>
         <v>1.6496606666666667</v>
       </c>
       <c r="Z8" s="26">
@@ -1676,9 +1711,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L9" s="30"/>
-      <c r="M9" s="15"/>
       <c r="N9" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O9" s="20"/>
@@ -1691,11 +1725,11 @@
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y9" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y9" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z9" s="26"/>
@@ -1720,58 +1754,98 @@
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" s="7">
         <v>44351</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14" t="e">
+      <c r="E10" s="20">
+        <f>4-1</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="16">
+        <f>3.2-1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G10" s="13">
+        <f>2.65-1</f>
+        <v>1.65</v>
+      </c>
+      <c r="H10" s="14">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14" t="e">
+        <v>2.2833333333333332</v>
+      </c>
+      <c r="I10" s="36">
+        <f>1.7-1</f>
+        <v>0.7</v>
+      </c>
+      <c r="J10" s="37">
+        <f>2-1</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.85</v>
       </c>
       <c r="L10" s="20"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="14" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="M10" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="N10" s="14">
+        <f>AVERAGE(L10:M10)*4</f>
+        <v>1</v>
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
+      <c r="T10" s="13">
+        <f>6.55%</f>
+        <v>6.5500000000000003E-2</v>
+      </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="14" t="e">
+      <c r="W10" s="13">
+        <f>(AVERAGE(R7, U7)/T7) * T10</f>
+        <v>0.1484793394140409</v>
+      </c>
+      <c r="X10" s="14">
+        <f t="shared" si="3"/>
+        <v>0.42795867882808181</v>
+      </c>
+      <c r="Y10" s="23">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y10" s="23" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="14" t="e">
+        <v>1.3825271351575457</v>
+      </c>
+      <c r="Z10" s="26">
+        <f>2.3-1</f>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="AA10" s="36">
+        <f>2.6-1</f>
+        <v>1.6</v>
+      </c>
+      <c r="AB10" s="20">
+        <f>2-1</f>
+        <v>1</v>
+      </c>
+      <c r="AC10" s="13">
+        <f>2-1</f>
+        <v>1</v>
+      </c>
+      <c r="AD10" s="13">
+        <f>1.5-1</f>
+        <v>0.5</v>
+      </c>
+      <c r="AE10" s="14">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF10" s="23" t="e">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="AF10" s="23">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1.2583333333333331</v>
       </c>
       <c r="AG10" s="4"/>
     </row>
@@ -1802,7 +1876,7 @@
       <c r="L11" s="20"/>
       <c r="M11" s="13"/>
       <c r="N11" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="20"/>
@@ -1815,11 +1889,11 @@
       <c r="V11" s="13"/>
       <c r="W11" s="13"/>
       <c r="X11" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y11" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y11" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z11" s="26"/>
@@ -1864,7 +1938,7 @@
       <c r="L12" s="20"/>
       <c r="M12" s="13"/>
       <c r="N12" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O12" s="20"/>
@@ -1877,11 +1951,11 @@
       <c r="V12" s="13"/>
       <c r="W12" s="13"/>
       <c r="X12" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y12" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y12" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z12" s="26"/>
@@ -1926,7 +2000,7 @@
       <c r="L13" s="20"/>
       <c r="M13" s="13"/>
       <c r="N13" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O13" s="20"/>
@@ -1939,11 +2013,11 @@
       <c r="V13" s="13"/>
       <c r="W13" s="13"/>
       <c r="X13" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y13" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y13" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z13" s="26"/>
@@ -2002,7 +2076,7 @@
       </c>
       <c r="M14" s="13"/>
       <c r="N14" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.5004</v>
       </c>
       <c r="O14" s="20"/>
@@ -2021,11 +2095,11 @@
       </c>
       <c r="W14" s="13"/>
       <c r="X14" s="14">
+        <f t="shared" si="3"/>
+        <v>2.2536537931034482</v>
+      </c>
+      <c r="Y14" s="23">
         <f t="shared" si="4"/>
-        <v>2.2536537931034482</v>
-      </c>
-      <c r="Y14" s="23">
-        <f t="shared" si="2"/>
         <v>2.9697747356321837</v>
       </c>
       <c r="Z14" s="26">
@@ -2082,7 +2156,7 @@
       <c r="L15" s="20"/>
       <c r="M15" s="13"/>
       <c r="N15" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O15" s="20"/>
@@ -2095,11 +2169,11 @@
       <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="X15" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y15" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y15" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z15" s="26"/>
@@ -2144,7 +2218,7 @@
       <c r="L16" s="20"/>
       <c r="M16" s="13"/>
       <c r="N16" s="14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="20"/>
@@ -2157,11 +2231,11 @@
       <c r="V16" s="13"/>
       <c r="W16" s="13"/>
       <c r="X16" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y16" s="23" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y16" s="23" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z16" s="26"/>
@@ -2225,7 +2299,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="N17" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.2400000000000002</v>
       </c>
       <c r="O17" s="20"/>
@@ -2240,11 +2314,11 @@
         <v>0.53</v>
       </c>
       <c r="X17" s="14">
+        <f t="shared" si="3"/>
+        <v>2.12</v>
+      </c>
+      <c r="Y17" s="23">
         <f t="shared" si="4"/>
-        <v>2.12</v>
-      </c>
-      <c r="Y17" s="23">
-        <f t="shared" si="2"/>
         <v>2.7490000000000001</v>
       </c>
       <c r="Z17" s="26">

</xml_diff>